<commit_message>
updated test case description
</commit_message>
<xml_diff>
--- a/tests/TestResult.xlsx
+++ b/tests/TestResult.xlsx
@@ -86,13 +86,18 @@
     <t>Failed-Unexpected status code: 400</t>
   </si>
   <si>
-    <t>normal update</t>
-  </si>
-  <si>
     <t>robot name updated</t>
   </si>
   <si>
     <t>'namechanger' user don't have access privileges to the specified Unit</t>
+  </si>
+  <si>
+    <t>normal update
+( 1. Find the Robot using the Unit Name, machine name and user name
+  2. check if the robot name is not the same as to-be robot name already
+  3. update the robot name to the new name
+  4. find the robot using the Unit name, machine name and user name again
+  5. confirm the robot name is the same as to-be robot name.)</t>
   </si>
 </sst>
 </file>
@@ -128,9 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +469,7 @@
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +566,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -570,12 +578,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>